<commit_message>
add proj id to simple file
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/file-success/EOHHS-075-06302020-simple-v1.xlsx
+++ b/tests/server/fixtures/file-success/EOHHS-075-06302020-simple-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmclaughlin/git/usdr/cares-reporter/tests/server/fixtures/file-success/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA41BD1-1138-B44A-9DCF-8DA1FFE3432A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F304DD16-B7D5-9C43-844D-F63AAD8A857F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="-18420" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1940" yWindow="-18420" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -1600,8 +1600,8 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1634,7 +1634,7 @@
         <v>324</v>
       </c>
       <c r="B2" s="29">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C2" s="59" t="s">
         <v>110</v>
@@ -11164,7 +11164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE547"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add a few contracts validations
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/file-success/EOHHS-075-06302020-simple-v1.xlsx
+++ b/tests/server/fixtures/file-success/EOHHS-075-06302020-simple-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmclaughlin/git/usdr/cares-reporter/tests/server/fixtures/file-success/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7757AB-9C7B-B24E-8955-07A1C9EFEE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DB2817-60D2-0240-9C44-322A07EA776E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1940" yWindow="-18420" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1601,7 +1601,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Small fixes and tweaks that will be useful soon.
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/file-success/EOHHS-075-06302020-simple-v1.xlsx
+++ b/tests/server/fixtures/file-success/EOHHS-075-06302020-simple-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmclaughlin/git/usdr/cares-reporter/tests/server/fixtures/file-success/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DB2817-60D2-0240-9C44-322A07EA776E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C5B589-17D8-8641-A531-09F5DC00FF2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="-18420" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1940" yWindow="-18420" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="338">
   <si>
     <t>Agency Code</t>
   </si>
@@ -772,9 +772,6 @@
     <t>35352</t>
   </si>
   <si>
-    <t>646</t>
-  </si>
-  <si>
     <t>967</t>
   </si>
   <si>
@@ -1073,7 +1070,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1136,6 +1133,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1287,7 +1290,7 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1378,6 +1381,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1600,7 +1604,7 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1623,15 +1627,15 @@
         <v>2</v>
       </c>
       <c r="E1" s="58" t="s">
+        <v>335</v>
+      </c>
+      <c r="F1" s="58" t="s">
         <v>336</v>
-      </c>
-      <c r="F1" s="58" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="59" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B2" s="29">
         <v>75</v>
@@ -2709,7 +2713,9 @@
   </sheetPr>
   <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3708,64 +3714,64 @@
     </row>
     <row r="2" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B2" s="54" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" s="55" t="s">
         <v>312</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="D2" s="54" t="s">
         <v>313</v>
-      </c>
-      <c r="D2" s="54" t="s">
-        <v>314</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B3" s="54" t="s">
+        <v>314</v>
+      </c>
+      <c r="C3" s="55" t="s">
         <v>315</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="D3" s="54" t="s">
         <v>316</v>
-      </c>
-      <c r="D3" s="54" t="s">
-        <v>317</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B4" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="55" t="s">
         <v>318</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="D4" s="54" t="s">
         <v>319</v>
-      </c>
-      <c r="D4" s="54" t="s">
-        <v>320</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5" s="54" t="s">
+        <v>320</v>
+      </c>
+      <c r="C5" s="55" t="s">
         <v>321</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="D5" s="54" t="s">
         <v>322</v>
-      </c>
-      <c r="D5" s="54" t="s">
-        <v>323</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -11164,8 +11170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE547"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11186,7 +11192,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>11</v>
@@ -11195,31 +11201,31 @@
         <v>12</v>
       </c>
       <c r="D1" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="27" t="s">
         <v>332</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>333</v>
       </c>
       <c r="H1" s="27" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="J1" s="27" t="s">
         <v>334</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>335</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L1" s="61" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
@@ -11241,330 +11247,360 @@
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
     </row>
-    <row r="2" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="57" t="s">
         <v>238</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E2" s="28"/>
       <c r="F2" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>202</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K2" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
         <v>239</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H3" s="28" t="s">
         <v>181</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J3" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K3" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="57" t="s">
         <v>240</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H4" s="28" t="s">
         <v>202</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J4" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K4" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="57" t="s">
         <v>241</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H5" s="28" t="s">
         <v>202</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J5" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="57" t="s">
-        <v>242</v>
+      <c r="K5" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="57"/>
+      <c r="B6" s="62">
+        <v>25460908</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>268</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
-      <c r="G6" s="28" t="s">
-        <v>283</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>294</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="57" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H7" s="28" t="s">
         <v>202</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J7" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K7" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="28" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>141</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J8" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K8" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="57" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E9" s="28"/>
       <c r="F9" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H9" s="28" t="s">
         <v>202</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J9" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K9" s="18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="57" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H10" s="28" t="s">
         <v>202</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J10" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K10" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="57" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>202</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J11" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K11" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="57" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>202</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J12" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K12" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>141</v>
       </c>
       <c r="I13" s="28" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J13" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="K13" s="13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="59"/>
+      <c r="K14" s="13"/>
+    </row>
+    <row r="15" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="13"/>
+    </row>
     <row r="16" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12112,7 +12148,7 @@
   <dimension ref="A1:AY984"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12281,13 +12317,13 @@
         <v>238</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E2" s="39">
         <v>1376</v>
@@ -12302,23 +12338,23 @@
         <v>44195</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M2" s="33" t="s">
         <v>202</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>113</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R2" s="5">
         <v>75</v>
@@ -12347,18 +12383,18 @@
       </c>
       <c r="AE2" s="5"/>
     </row>
-    <row r="3" spans="1:51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="34" t="s">
-        <v>242</v>
+    <row r="3" spans="1:51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="62">
+        <v>25460908</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E3" s="40">
         <v>537579</v>
@@ -12373,24 +12409,24 @@
         <v>44195</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J3" s="34"/>
       <c r="K3" s="5"/>
       <c r="L3" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M3" s="34" t="s">
         <v>164</v>
       </c>
       <c r="N3" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>113</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R3" s="6">
         <v>75</v>
@@ -12424,16 +12460,16 @@
     </row>
     <row r="4" spans="1:51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E4" s="39">
         <v>27620</v>
@@ -12448,24 +12484,24 @@
         <v>44195</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J4" s="33"/>
       <c r="K4" s="5"/>
       <c r="L4" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M4" s="33" t="s">
         <v>202</v>
       </c>
       <c r="N4" s="33" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>113</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R4" s="6">
         <v>75</v>
@@ -19694,7 +19730,7 @@
         <v>239</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>124</v>
@@ -19712,18 +19748,18 @@
         <v>44195</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
       <c r="L2" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M2" s="33" t="s">
         <v>181</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O2" s="43" t="s">
         <v>113</v>
@@ -19741,7 +19777,7 @@
         <v>43969.648842592593</v>
       </c>
       <c r="W2" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="X2" s="41">
         <v>585520</v>
@@ -36869,10 +36905,10 @@
         <v>241</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D2" s="33">
         <v>50311.8</v>
@@ -36884,28 +36920,28 @@
         <v>44104</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K2" s="33" t="s">
         <v>202</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M2" s="33" t="s">
         <v>113</v>
       </c>
       <c r="O2" s="43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P2" s="33">
         <v>50311.8</v>
@@ -36922,13 +36958,13 @@
     </row>
     <row r="3" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D3" s="34">
         <v>50529.599999999999</v>
@@ -36940,26 +36976,26 @@
         <v>44104</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H3" s="34"/>
       <c r="I3" s="34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K3" s="34" t="s">
         <v>202</v>
       </c>
       <c r="L3" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M3" s="34" t="s">
         <v>113</v>
       </c>
       <c r="O3" s="43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P3" s="34">
         <v>50529.599999999999</v>
@@ -36979,10 +37015,10 @@
         <v>240</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D4" s="33">
         <v>50856.3</v>
@@ -36994,28 +37030,28 @@
         <v>44104</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K4" s="33" t="s">
         <v>202</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M4" s="33" t="s">
         <v>113</v>
       </c>
       <c r="O4" s="43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P4" s="33">
         <v>50856.3</v>
@@ -39368,13 +39404,13 @@
     </row>
     <row r="2" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="53" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D2" s="41">
         <v>32416.32</v>
@@ -39383,10 +39419,10 @@
         <v>43987.643125000002</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H2">
         <v>75</v>
@@ -46455,10 +46491,10 @@
     </row>
     <row r="2" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C2" s="48">
         <v>21011844.77</v>
@@ -46497,10 +46533,10 @@
     </row>
     <row r="3" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="47" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C3" s="49">
         <v>15782137.59</v>
@@ -46537,10 +46573,10 @@
     </row>
     <row r="4" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C4" s="48">
         <v>9647704.7699999996</v>
@@ -53583,7 +53619,7 @@
         <v>75</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D3" s="56">
         <v>2163121.9700000002</v>

</xml_diff>